<commit_message>
correcção do excel areia branca
correcção do excel areia branca
</commit_message>
<xml_diff>
--- a/data/areia_branca.xlsx
+++ b/data/areia_branca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Dropbox\Urban Modeling Dashboard\Development seed\CEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52A2CD4-7A3B-4906-B76E-F0D1CACC0F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABD0C32-372E-4EF1-8B49-FFB7EFED12F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,15 +326,9 @@
     <t>Name*</t>
   </si>
   <si>
-    <t>Lisbon Building Data</t>
-  </si>
-  <si>
     <t>Description*</t>
   </si>
   <si>
-    <t>Building energy consumption and intervention scenarios. The modelling considered  data from Census, 2011 and Census, 2021; Decree-law: 80/2006. The modelling was performed by IN+, IST using CEA software on 2023.</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
@@ -597,6 +591,12 @@
   </si>
   <si>
     <t>To define</t>
+  </si>
+  <si>
+    <t>Areia Branca</t>
+  </si>
+  <si>
+    <t>Building energy consumption, impact and cost. Dummy values</t>
   </si>
 </sst>
 </file>
@@ -962,7 +962,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M17:M18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,41 +972,41 @@
         <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -1014,15 +1014,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2714,7 +2714,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2851,10 +2851,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -2862,10 +2862,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -2873,10 +2873,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2895,10 +2895,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2906,10 +2906,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2917,10 +2917,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2928,10 +2928,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2939,10 +2939,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2950,10 +2950,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -2961,10 +2961,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -2972,10 +2972,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -2983,10 +2983,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -2994,10 +2994,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -3005,10 +3005,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -3016,10 +3016,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -3027,10 +3027,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -3038,10 +3038,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -3049,10 +3049,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -3082,10 +3082,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -3093,10 +3093,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -3104,10 +3104,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -3115,10 +3115,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -3159,10 +3159,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B44" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -3192,10 +3192,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -3203,10 +3203,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B47" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -3225,10 +3225,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -3236,10 +3236,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B49" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B50" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -3269,10 +3269,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B52" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>

</xml_diff>